<commit_message>
Added folio ids to import PI
</commit_message>
<xml_diff>
--- a/public/sample_uploads/portfolio_investments2.xlsx
+++ b/public/sample_uploads/portfolio_investments2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t xml:space="preserve">Fund</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">Custom Field 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excused Folio Ids</t>
   </si>
   <si>
     <t xml:space="preserve">SAAS Fund</t>
@@ -90,7 +93,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -132,6 +135,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -197,20 +206,28 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -465,124 +482,127 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1013" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1013" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="n">
         <v>43831</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>2000000</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>20000</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="n">
         <v>43831</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>1000000</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>-10000</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>